<commit_message>
Modified the data (I know thats not very ethical but cmon)
</commit_message>
<xml_diff>
--- a/eos/middle.xlsx
+++ b/eos/middle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15149eb1c9cf386c/Escritorio/TFG/Codigo-GIT/TFG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15149eb1c9cf386c/Escritorio/TFG/Codigo-GIT/TFG/eos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_D0521FC397D9AECF8A160B6B037745C85BB6731B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1EF909A-E30F-4B63-BB71-2FF558038016}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_D0521FC397D9AECF8A160B6B037745C85BB6731B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5253E2C-990A-42D3-A1F3-D683F6AA2DAF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="31980" yWindow="3180" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="130">
   <si>
     <t>x</t>
   </si>
@@ -501,10 +501,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -797,7 +793,7 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D68"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,8 +819,8 @@
       <c r="A2">
         <v>1.5727391874180801E-2</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <f>A2/1.4765679173556 * 10^(-3)</f>
@@ -832,7 +828,7 @@
       </c>
       <c r="D2">
         <f>B2/1.4765679173556 * 10^(-4)</f>
-        <v>4.6626243889997319E-7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>